<commit_message>
Update logic to read info from excel based on existing Studio languages
</commit_message>
<xml_diff>
--- a/Be GlobalV4 Translation Provider/Sdl.Community.BeGlobalV4.Provider/Resources/MTLanguageCodes.xlsx
+++ b/Be GlobalV4 Translation Provider/Sdl.Community.BeGlobalV4.Provider/Resources/MTLanguageCodes.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$610</definedName>
     <definedName name="unifiedCodes" localSheetId="0">Sheet1!$A$2:$D$610</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="1399">
   <si>
     <t>Language</t>
   </si>
@@ -4114,6 +4114,123 @@
   </si>
   <si>
     <t>zul</t>
+  </si>
+  <si>
+    <t>Edo</t>
+  </si>
+  <si>
+    <t>bin-NG</t>
+  </si>
+  <si>
+    <t>ce-RU</t>
+  </si>
+  <si>
+    <t>en-ID</t>
+  </si>
+  <si>
+    <t>fr-029</t>
+  </si>
+  <si>
+    <t>Ibibio</t>
+  </si>
+  <si>
+    <t>ibb-NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javanese </t>
+  </si>
+  <si>
+    <t>Javanese, Indonesia</t>
+  </si>
+  <si>
+    <t>jv-Java-ID</t>
+  </si>
+  <si>
+    <t>Kanuri</t>
+  </si>
+  <si>
+    <t>kr-NG</t>
+  </si>
+  <si>
+    <t>Devanagari, India</t>
+  </si>
+  <si>
+    <t>ks-Deva-IN</t>
+  </si>
+  <si>
+    <t>la-001</t>
+  </si>
+  <si>
+    <t>Manipuri</t>
+  </si>
+  <si>
+    <t>mni-IN</t>
+  </si>
+  <si>
+    <t>Latin, Singapore</t>
+  </si>
+  <si>
+    <t>ms-SG</t>
+  </si>
+  <si>
+    <t>Papiamento</t>
+  </si>
+  <si>
+    <t>pap-029</t>
+  </si>
+  <si>
+    <t>Prussian</t>
+  </si>
+  <si>
+    <t>prg-001</t>
+  </si>
+  <si>
+    <t>sd-Deva-IN</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>sq-XK</t>
+  </si>
+  <si>
+    <t>Cyrillic, Kosovo</t>
+  </si>
+  <si>
+    <t>sr-Cyrl-XK</t>
+  </si>
+  <si>
+    <t>Latin, Kosovo</t>
+  </si>
+  <si>
+    <t>sr-Latn-XK</t>
+  </si>
+  <si>
+    <t>sw-CD</t>
+  </si>
+  <si>
+    <t>Arabic, Morocco</t>
+  </si>
+  <si>
+    <t>tzm-Arab-MA</t>
+  </si>
+  <si>
+    <t>Yiddish</t>
+  </si>
+  <si>
+    <t>yi-001</t>
+  </si>
+  <si>
+    <t>Simplified Han, Hong Kong SAR</t>
+  </si>
+  <si>
+    <t>zh-Hans-HK</t>
+  </si>
+  <si>
+    <t>Simplified Han, Macao SAR</t>
+  </si>
+  <si>
+    <t>zh-Hans-MO</t>
   </si>
 </sst>
 </file>
@@ -4480,18 +4597,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F610"/>
+  <dimension ref="A1:F632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A611" sqref="A611:XFD611"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="26.75" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13048,6 +13165,248 @@
         <v>1359</v>
       </c>
     </row>
+    <row r="611" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B611" t="s">
+        <v>429</v>
+      </c>
+      <c r="C611" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="612" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>214</v>
+      </c>
+      <c r="B612" t="s">
+        <v>147</v>
+      </c>
+      <c r="C612" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>310</v>
+      </c>
+      <c r="B613" t="s">
+        <v>699</v>
+      </c>
+      <c r="C613" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>530</v>
+      </c>
+      <c r="B614" t="s">
+        <v>313</v>
+      </c>
+      <c r="C614" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B615" t="s">
+        <v>429</v>
+      </c>
+      <c r="C615" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B616" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C616" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="617" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B617" t="s">
+        <v>429</v>
+      </c>
+      <c r="C617" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="618" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>760</v>
+      </c>
+      <c r="B618" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C618" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="619" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>133</v>
+      </c>
+      <c r="B619" t="s">
+        <v>45</v>
+      </c>
+      <c r="C619" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="620" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B620" t="s">
+        <v>110</v>
+      </c>
+      <c r="C620" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="621" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>862</v>
+      </c>
+      <c r="B621" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C621" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="622" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B622" t="s">
+        <v>313</v>
+      </c>
+      <c r="C622" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B623" t="s">
+        <v>45</v>
+      </c>
+      <c r="C623" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B624" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C624" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>27</v>
+      </c>
+      <c r="B625" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C625" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B626" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C626" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B627" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C627" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>779</v>
+      </c>
+      <c r="B628" t="s">
+        <v>249</v>
+      </c>
+      <c r="C628" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>205</v>
+      </c>
+      <c r="B629" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C629" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B630" t="s">
+        <v>45</v>
+      </c>
+      <c r="C630" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
+        <v>241</v>
+      </c>
+      <c r="B631" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C631" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>241</v>
+      </c>
+      <c r="B632" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C632" t="s">
+        <v>1398</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D610"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new update MTLanguagesCodes file
</commit_message>
<xml_diff>
--- a/Be GlobalV4 Translation Provider/Sdl.Community.BeGlobalV4.Provider/Resources/MTLanguageCodes.xlsx
+++ b/Be GlobalV4 Translation Provider/Sdl.Community.BeGlobalV4.Provider/Resources/MTLanguageCodes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TradosStudio_Plugins\BeGlobal\LanguageMappings_Feature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcaputa\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="465" windowWidth="19200" windowHeight="21135"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2510" uniqueCount="1399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2532" uniqueCount="1399">
   <si>
     <t>Language</t>
   </si>
@@ -4600,7 +4594,8 @@
   <dimension ref="A1:F632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="A611" sqref="A611:XFD611"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4608,7 +4603,7 @@
     <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="26.75" customWidth="1"/>
+    <col min="4" max="4" width="26.625" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13175,6 +13170,9 @@
       <c r="C611" t="s">
         <v>1361</v>
       </c>
+      <c r="D611" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="612" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
@@ -13186,6 +13184,9 @@
       <c r="C612" t="s">
         <v>1362</v>
       </c>
+      <c r="D612" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="613" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
@@ -13197,6 +13198,9 @@
       <c r="C613" t="s">
         <v>1363</v>
       </c>
+      <c r="D613" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="614" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
@@ -13208,6 +13212,9 @@
       <c r="C614" t="s">
         <v>1364</v>
       </c>
+      <c r="D614" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="615" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
@@ -13219,6 +13226,9 @@
       <c r="C615" t="s">
         <v>1366</v>
       </c>
+      <c r="D615" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="616" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
@@ -13230,6 +13240,9 @@
       <c r="C616" t="s">
         <v>1369</v>
       </c>
+      <c r="D616" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="617" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
@@ -13241,6 +13254,9 @@
       <c r="C617" t="s">
         <v>1371</v>
       </c>
+      <c r="D617" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="618" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
@@ -13252,6 +13268,9 @@
       <c r="C618" t="s">
         <v>1373</v>
       </c>
+      <c r="D618" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="619" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
@@ -13263,6 +13282,9 @@
       <c r="C619" t="s">
         <v>1374</v>
       </c>
+      <c r="D619" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="620" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
@@ -13274,6 +13296,9 @@
       <c r="C620" t="s">
         <v>1376</v>
       </c>
+      <c r="D620" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="621" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
@@ -13285,6 +13310,9 @@
       <c r="C621" t="s">
         <v>1378</v>
       </c>
+      <c r="D621" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="622" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
@@ -13296,6 +13324,9 @@
       <c r="C622" t="s">
         <v>1380</v>
       </c>
+      <c r="D622" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="623" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
@@ -13307,6 +13338,9 @@
       <c r="C623" t="s">
         <v>1382</v>
       </c>
+      <c r="D623" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="624" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
@@ -13318,8 +13352,11 @@
       <c r="C624" t="s">
         <v>1383</v>
       </c>
-    </row>
-    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D624" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
         <v>27</v>
       </c>
@@ -13329,8 +13366,11 @@
       <c r="C625" t="s">
         <v>1385</v>
       </c>
-    </row>
-    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D625" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="626" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
         <v>1103</v>
       </c>
@@ -13340,8 +13380,11 @@
       <c r="C626" t="s">
         <v>1387</v>
       </c>
-    </row>
-    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D626" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
         <v>1103</v>
       </c>
@@ -13351,8 +13394,11 @@
       <c r="C627" t="s">
         <v>1389</v>
       </c>
-    </row>
-    <row r="628" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D627" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
         <v>779</v>
       </c>
@@ -13362,8 +13408,11 @@
       <c r="C628" t="s">
         <v>1390</v>
       </c>
-    </row>
-    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D628" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
         <v>205</v>
       </c>
@@ -13373,8 +13422,11 @@
       <c r="C629" t="s">
         <v>1392</v>
       </c>
-    </row>
-    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D629" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="630" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
         <v>1393</v>
       </c>
@@ -13384,8 +13436,11 @@
       <c r="C630" t="s">
         <v>1394</v>
       </c>
-    </row>
-    <row r="631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D630" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
         <v>241</v>
       </c>
@@ -13395,8 +13450,11 @@
       <c r="C631" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="632" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D631" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="632" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
         <v>241</v>
       </c>
@@ -13405,6 +13463,9 @@
       </c>
       <c r="C632" t="s">
         <v>1398</v>
+      </c>
+      <c r="D632" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Save language mappings configuration when user add the provider using project creation wizard. Update MT codes files with the latest codes received from LS. Update plugin version
</commit_message>
<xml_diff>
--- a/Be GlobalV4 Translation Provider/Sdl.Community.BeGlobalV4.Provider/Resources/MTLanguageCodes.xlsx
+++ b/Be GlobalV4 Translation Provider/Sdl.Community.BeGlobalV4.Provider/Resources/MTLanguageCodes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="1399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2466" uniqueCount="1421">
   <si>
     <t>Language</t>
   </si>
@@ -4225,13 +4225,79 @@
   </si>
   <si>
     <t>Simplified</t>
+  </si>
+  <si>
+    <t>srp</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>esx</t>
+  </si>
+  <si>
+    <t>esb</t>
+  </si>
+  <si>
+    <t>esc</t>
+  </si>
+  <si>
+    <t>ese</t>
+  </si>
+  <si>
+    <t>esg</t>
+  </si>
+  <si>
+    <t>esh</t>
+  </si>
+  <si>
+    <t>esi</t>
+  </si>
+  <si>
+    <t>esj</t>
+  </si>
+  <si>
+    <t>esd</t>
+  </si>
+  <si>
+    <t>esn</t>
+  </si>
+  <si>
+    <t>esp</t>
+  </si>
+  <si>
+    <t>esy</t>
+  </si>
+  <si>
+    <t>esr</t>
+  </si>
+  <si>
+    <t>esw</t>
+  </si>
+  <si>
+    <t>eso</t>
+  </si>
+  <si>
+    <t>esq</t>
+  </si>
+  <si>
+    <t>esu</t>
+  </si>
+  <si>
+    <t>esv</t>
+  </si>
+  <si>
+    <t>esz</t>
+  </si>
+  <si>
+    <t>ptp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4245,6 +4311,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4268,7 +4341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -4277,6 +4350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4594,8 +4668,8 @@
   <dimension ref="A1:F632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A612" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A633" sqref="A633:XFD633"/>
+      <pane ySplit="1" topLeftCell="A421" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E439" sqref="E439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6585,7 +6659,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>294</v>
       </c>
@@ -6598,8 +6672,11 @@
       <c r="D145" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>294</v>
       </c>
@@ -6613,7 +6690,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>294</v>
       </c>
@@ -6627,7 +6704,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>294</v>
       </c>
@@ -6641,7 +6718,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>294</v>
       </c>
@@ -6655,7 +6732,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>294</v>
       </c>
@@ -6669,7 +6746,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>294</v>
       </c>
@@ -6683,7 +6760,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>294</v>
       </c>
@@ -6697,7 +6774,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>294</v>
       </c>
@@ -6711,7 +6788,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>294</v>
       </c>
@@ -6725,7 +6802,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>294</v>
       </c>
@@ -6739,7 +6816,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>294</v>
       </c>
@@ -6753,7 +6830,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>294</v>
       </c>
@@ -6767,7 +6844,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>294</v>
       </c>
@@ -6781,7 +6858,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>294</v>
       </c>
@@ -6795,7 +6872,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>294</v>
       </c>
@@ -7481,7 +7558,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>294</v>
       </c>
@@ -7495,7 +7572,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>294</v>
       </c>
@@ -7508,8 +7585,11 @@
       <c r="D210" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>294</v>
       </c>
@@ -7523,7 +7603,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>294</v>
       </c>
@@ -7537,7 +7617,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>294</v>
       </c>
@@ -7551,7 +7631,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>294</v>
       </c>
@@ -7565,7 +7645,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>294</v>
       </c>
@@ -7579,7 +7659,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>294</v>
       </c>
@@ -7593,7 +7673,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>294</v>
       </c>
@@ -7607,7 +7687,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>294</v>
       </c>
@@ -7621,7 +7701,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>484</v>
       </c>
@@ -7635,7 +7715,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>487</v>
       </c>
@@ -7649,7 +7729,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>491</v>
       </c>
@@ -7663,7 +7743,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>491</v>
       </c>
@@ -7677,7 +7757,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>496</v>
       </c>
@@ -7691,7 +7771,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>499</v>
       </c>
@@ -10530,7 +10610,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>954</v>
       </c>
@@ -10544,7 +10624,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>954</v>
       </c>
@@ -10558,7 +10638,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>954</v>
       </c>
@@ -10572,7 +10652,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>954</v>
       </c>
@@ -10586,7 +10666,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>954</v>
       </c>
@@ -10600,7 +10680,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>954</v>
       </c>
@@ -10614,7 +10694,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>954</v>
       </c>
@@ -10627,8 +10707,11 @@
       <c r="D439" t="s">
         <v>956</v>
       </c>
-    </row>
-    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E439" s="3" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>954</v>
       </c>
@@ -10642,7 +10725,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>954</v>
       </c>
@@ -10656,7 +10739,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>973</v>
       </c>
@@ -10667,7 +10750,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>973</v>
       </c>
@@ -10678,7 +10761,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>973</v>
       </c>
@@ -10689,7 +10772,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>980</v>
       </c>
@@ -10703,7 +10786,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>980</v>
       </c>
@@ -10717,7 +10800,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>980</v>
       </c>
@@ -10731,7 +10814,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>986</v>
       </c>
@@ -11169,7 +11252,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>1055</v>
       </c>
@@ -11180,7 +11263,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>1067</v>
       </c>
@@ -11194,7 +11277,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>1067</v>
       </c>
@@ -11208,7 +11291,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>1067</v>
       </c>
@@ -11222,7 +11305,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>1067</v>
       </c>
@@ -11236,7 +11319,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>1067</v>
       </c>
@@ -11249,8 +11332,11 @@
       <c r="D486" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E486" s="3" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>1067</v>
       </c>
@@ -11263,8 +11349,11 @@
       <c r="D487" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E487" s="3" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>1067</v>
       </c>
@@ -11277,8 +11366,11 @@
       <c r="D488" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E488" s="3" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>1067</v>
       </c>
@@ -11291,8 +11383,11 @@
       <c r="D489" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E489" s="3" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>1067</v>
       </c>
@@ -11306,7 +11401,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>1067</v>
       </c>
@@ -11319,8 +11414,11 @@
       <c r="D491" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E491" s="3" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>1070</v>
       </c>
@@ -11331,7 +11429,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>1072</v>
       </c>
@@ -11342,7 +11440,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>1072</v>
       </c>
@@ -11353,7 +11451,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="495" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>1075</v>
       </c>
@@ -11364,7 +11462,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>1077</v>
       </c>
@@ -11618,6 +11716,9 @@
       <c r="D513" t="s">
         <v>1113</v>
       </c>
+      <c r="E513" s="3" t="s">
+        <v>1402</v>
+      </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
@@ -11660,6 +11761,9 @@
       <c r="D516" t="s">
         <v>1113</v>
       </c>
+      <c r="E516" s="4" t="s">
+        <v>1407</v>
+      </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
@@ -11674,6 +11778,9 @@
       <c r="D517" t="s">
         <v>1113</v>
       </c>
+      <c r="E517" s="3" t="s">
+        <v>1403</v>
+      </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
@@ -11688,6 +11795,9 @@
       <c r="D518" t="s">
         <v>1113</v>
       </c>
+      <c r="E518" s="3" t="s">
+        <v>1408</v>
+      </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
@@ -11716,6 +11826,9 @@
       <c r="D520" t="s">
         <v>1113</v>
       </c>
+      <c r="E520" s="3" t="s">
+        <v>1409</v>
+      </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
@@ -11730,6 +11843,9 @@
       <c r="D521" t="s">
         <v>1113</v>
       </c>
+      <c r="E521" s="3" t="s">
+        <v>1404</v>
+      </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
@@ -11789,6 +11905,9 @@
       <c r="D525" t="s">
         <v>1113</v>
       </c>
+      <c r="E525" s="3" t="s">
+        <v>1405</v>
+      </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
@@ -11803,6 +11922,9 @@
       <c r="D526" t="s">
         <v>1113</v>
       </c>
+      <c r="E526" s="3" t="s">
+        <v>1406</v>
+      </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
@@ -11834,8 +11956,11 @@
       <c r="D528" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="529" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E528" s="3" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>1110</v>
       </c>
@@ -11848,8 +11973,11 @@
       <c r="D529" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="530" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E529" s="3" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="530" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>1110</v>
       </c>
@@ -11862,8 +11990,11 @@
       <c r="D530" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="531" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E530" s="3" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>1110</v>
       </c>
@@ -11877,7 +12008,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="532" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>1110</v>
       </c>
@@ -11890,8 +12021,11 @@
       <c r="D532" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="533" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E532" s="3" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="533" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>1110</v>
       </c>
@@ -11904,8 +12038,11 @@
       <c r="D533" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="534" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E533" s="3" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>1110</v>
       </c>
@@ -11918,8 +12055,11 @@
       <c r="D534" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="535" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E534" s="3" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>1110</v>
       </c>
@@ -11932,8 +12072,11 @@
       <c r="D535" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E535" s="3" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>1110</v>
       </c>
@@ -11946,8 +12089,11 @@
       <c r="D536" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E536" s="3" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>1110</v>
       </c>
@@ -11960,8 +12106,11 @@
       <c r="D537" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E537" s="3" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>1110</v>
       </c>
@@ -11974,8 +12123,11 @@
       <c r="D538" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E538" s="3" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>1110</v>
       </c>
@@ -11988,8 +12140,11 @@
       <c r="D539" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E539" s="3" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>1110</v>
       </c>
@@ -12002,8 +12157,11 @@
       <c r="D540" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="541" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E540" s="3" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>1162</v>
       </c>
@@ -12014,7 +12172,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="542" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>1162</v>
       </c>
@@ -12025,7 +12183,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="543" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>1166</v>
       </c>
@@ -12039,7 +12197,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="544" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>1390</v>
       </c>
@@ -12895,7 +13053,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="609" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A609" t="s">
         <v>1312</v>
       </c>
@@ -12906,7 +13064,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="610" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
         <v>1371</v>
       </c>
@@ -12920,7 +13078,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="611" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
         <v>1316</v>
       </c>
@@ -12931,7 +13089,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="612" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
         <v>205</v>
       </c>
@@ -12942,7 +13100,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="613" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
         <v>294</v>
       </c>
@@ -12952,8 +13110,14 @@
       <c r="C613" t="s">
         <v>1319</v>
       </c>
-    </row>
-    <row r="614" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D613" t="s">
+        <v>296</v>
+      </c>
+      <c r="E613" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="614" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
         <v>514</v>
       </c>
@@ -12964,7 +13128,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="615" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
         <v>1321</v>
       </c>
@@ -12975,7 +13139,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="616" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
         <v>714</v>
       </c>
@@ -12986,7 +13150,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="617" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
         <v>1325</v>
       </c>
@@ -12997,7 +13161,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="618" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
         <v>739</v>
       </c>
@@ -13008,7 +13172,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="619" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
         <v>129</v>
       </c>
@@ -13019,7 +13183,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="620" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
         <v>1330</v>
       </c>
@@ -13030,7 +13194,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="621" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
         <v>840</v>
       </c>
@@ -13041,7 +13205,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="622" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
         <v>1334</v>
       </c>
@@ -13052,7 +13216,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="623" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
         <v>1336</v>
       </c>
@@ -13063,7 +13227,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="624" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
         <v>1081</v>
       </c>
@@ -13074,7 +13238,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="625" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
         <v>26</v>
       </c>
@@ -13085,7 +13249,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="626" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
         <v>1067</v>
       </c>
@@ -13099,7 +13263,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="627" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
         <v>1067</v>
       </c>
@@ -13112,8 +13276,11 @@
       <c r="D627" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="628" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E627" s="3" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="628" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
         <v>758</v>
       </c>
@@ -13124,7 +13291,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="629" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
         <v>196</v>
       </c>
@@ -13135,7 +13302,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="630" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
         <v>1348</v>
       </c>
@@ -13146,7 +13313,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="631" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="631" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
         <v>227</v>
       </c>
@@ -13159,8 +13326,11 @@
       <c r="D631" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="632" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E631" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="632" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
         <v>227</v>
       </c>

</xml_diff>